<commit_message>
adding readme and updates for yesterday to tracker
</commit_message>
<xml_diff>
--- a/visualize_yourself/factor_tracker/factor_tracker_v1.xlsx
+++ b/visualize_yourself/factor_tracker/factor_tracker_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zack/dat203_ccac/visualize_yourself/factor_tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9148823C-E556-9644-B1E0-3D6035E86E38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C21D159-1772-8C4D-919F-EC257E696272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{A1BA6AF8-65AC-1A49-9373-6E2A5D38BDA9}"/>
+    <workbookView xWindow="28500" yWindow="660" windowWidth="25440" windowHeight="15000" xr2:uid="{A1BA6AF8-65AC-1A49-9373-6E2A5D38BDA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -452,42 +452,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -507,6 +480,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -516,8 +492,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -527,7 +501,33 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E573A9E-18A6-FA42-859D-81536E76F4F6}">
   <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -864,662 +864,694 @@
   <sheetData>
     <row r="1" spans="1:21" ht="17" thickBot="1"/>
     <row r="2" spans="1:21" ht="17" thickBot="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="31" t="s">
+      <c r="B2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="26" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="26" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="27"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="26" t="s">
+      <c r="M2" s="21"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="26" t="s">
+      <c r="P2" s="21"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="27"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="20"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="11"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="25" t="s">
+      <c r="O3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="25" t="s">
+      <c r="Q3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="S3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="29" t="s">
+      <c r="T3" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="19">
+      <c r="A4" s="10">
         <v>44103</v>
       </c>
-      <c r="B4" s="22">
-        <v>0</v>
-      </c>
-      <c r="C4" s="13">
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
         <v>20</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="13">
         <v>15</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="14">
         <v>45</v>
       </c>
-      <c r="F4" s="22">
-        <v>0</v>
-      </c>
-      <c r="G4" s="23">
-        <v>0</v>
-      </c>
-      <c r="H4" s="22">
+      <c r="F4" s="13">
+        <v>0</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
         <v>1</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="7">
         <v>2</v>
       </c>
-      <c r="J4" s="22">
-        <v>0</v>
-      </c>
-      <c r="K4" s="13">
+      <c r="J4" s="13">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
         <v>3</v>
       </c>
-      <c r="L4" s="22">
+      <c r="L4" s="13">
         <v>1</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="7">
         <v>2</v>
       </c>
-      <c r="N4" s="22">
-        <v>0</v>
-      </c>
-      <c r="O4" s="22">
+      <c r="N4" s="13">
+        <v>0</v>
+      </c>
+      <c r="O4" s="13">
         <v>2</v>
       </c>
-      <c r="P4" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="24">
+      <c r="P4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="15">
         <v>0.85416666666666663</v>
       </c>
-      <c r="R4" s="13">
+      <c r="R4" s="7">
         <v>180</v>
       </c>
-      <c r="S4" s="13">
+      <c r="S4" s="7">
         <v>90</v>
       </c>
-      <c r="T4" s="13">
+      <c r="T4" s="7">
         <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="19">
+      <c r="A5" s="10">
         <v>44104</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="13">
         <v>120</v>
       </c>
-      <c r="C5" s="13">
-        <v>0</v>
-      </c>
-      <c r="D5" s="22">
-        <v>0</v>
-      </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-      <c r="F5" s="22">
-        <v>0</v>
-      </c>
-      <c r="G5" s="23">
-        <v>0</v>
-      </c>
-      <c r="H5" s="22">
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
         <v>2</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="7">
         <v>2</v>
       </c>
-      <c r="J5" s="22">
-        <v>0</v>
-      </c>
-      <c r="K5" s="13">
+      <c r="J5" s="13">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
         <v>2</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="13">
         <v>1</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="7">
         <v>2</v>
       </c>
-      <c r="N5" s="22">
-        <v>0</v>
-      </c>
-      <c r="O5" s="22">
+      <c r="N5" s="13">
+        <v>0</v>
+      </c>
+      <c r="O5" s="13">
         <v>3</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="7">
         <v>1</v>
       </c>
-      <c r="Q5" s="24">
+      <c r="Q5" s="15">
         <v>0.83333333333333337</v>
       </c>
-      <c r="R5" s="13">
+      <c r="R5" s="7">
         <v>150</v>
       </c>
-      <c r="S5" s="13">
+      <c r="S5" s="7">
         <v>100</v>
       </c>
-      <c r="T5" s="13">
+      <c r="T5" s="7">
         <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="19">
+      <c r="A6" s="10">
         <v>44105</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="13">
         <v>240</v>
       </c>
-      <c r="C6" s="13">
-        <v>0</v>
-      </c>
-      <c r="D6" s="22">
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13">
         <v>25</v>
       </c>
-      <c r="E6" s="23">
-        <v>0</v>
-      </c>
-      <c r="F6" s="22">
-        <v>0</v>
-      </c>
-      <c r="G6" s="23">
-        <v>0</v>
-      </c>
-      <c r="H6" s="22">
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
         <v>2</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="7">
         <v>3</v>
       </c>
-      <c r="J6" s="22">
-        <v>0</v>
-      </c>
-      <c r="K6" s="13">
+      <c r="J6" s="13">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
         <v>1</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="13">
         <v>2</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="7">
         <v>3</v>
       </c>
-      <c r="N6" s="22">
-        <v>0</v>
-      </c>
-      <c r="O6" s="22">
+      <c r="N6" s="13">
+        <v>0</v>
+      </c>
+      <c r="O6" s="13">
         <v>2</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="7">
         <v>1</v>
       </c>
-      <c r="Q6" s="24">
+      <c r="Q6" s="15">
         <v>0.84722222222222221</v>
       </c>
-      <c r="R6" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S6" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="T6" s="13" t="s">
+      <c r="R6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T6" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="19">
+      <c r="A7" s="10">
         <v>44106</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="13">
         <v>240</v>
       </c>
-      <c r="C7" s="13">
-        <v>0</v>
-      </c>
-      <c r="D7" s="22">
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="13">
         <v>30</v>
       </c>
-      <c r="E7" s="23">
-        <v>0</v>
-      </c>
-      <c r="F7" s="22">
-        <v>0</v>
-      </c>
-      <c r="G7" s="23">
-        <v>0</v>
-      </c>
-      <c r="H7" s="22">
+      <c r="E7" s="14">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0</v>
+      </c>
+      <c r="G7" s="14">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13">
         <v>3</v>
       </c>
-      <c r="I7" s="13">
-        <v>0</v>
-      </c>
-      <c r="J7" s="22">
-        <v>0</v>
-      </c>
-      <c r="K7" s="13">
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="13">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
         <v>1</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="13">
         <v>2</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="7">
         <v>3</v>
       </c>
-      <c r="N7" s="22">
-        <v>0</v>
-      </c>
-      <c r="O7" s="22">
+      <c r="N7" s="13">
+        <v>0</v>
+      </c>
+      <c r="O7" s="13">
         <v>2</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="7">
         <v>1</v>
       </c>
-      <c r="Q7" s="24">
+      <c r="Q7" s="15">
         <v>0.83333333333333337</v>
       </c>
-      <c r="R7" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S7" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="T7" s="13" t="s">
+      <c r="R7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T7" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="19">
+      <c r="A8" s="10">
         <v>44107</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="13">
         <v>180</v>
       </c>
-      <c r="C8" s="13">
-        <v>0</v>
-      </c>
-      <c r="D8" s="22">
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="13">
         <v>45</v>
       </c>
-      <c r="E8" s="23">
-        <v>0</v>
-      </c>
-      <c r="F8" s="22">
-        <v>0</v>
-      </c>
-      <c r="G8" s="23">
-        <v>0</v>
-      </c>
-      <c r="H8" s="22">
+      <c r="E8" s="14">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
         <v>2</v>
       </c>
-      <c r="I8" s="13">
-        <v>0</v>
-      </c>
-      <c r="J8" s="22">
-        <v>0</v>
-      </c>
-      <c r="K8" s="13">
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
         <v>3</v>
       </c>
-      <c r="L8" s="22">
+      <c r="L8" s="13">
         <v>1</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="7">
         <v>2</v>
       </c>
-      <c r="N8" s="22">
-        <v>0</v>
-      </c>
-      <c r="O8" s="22">
+      <c r="N8" s="13">
+        <v>0</v>
+      </c>
+      <c r="O8" s="13">
         <v>4</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="7">
         <v>1</v>
       </c>
-      <c r="Q8" s="24">
+      <c r="Q8" s="15">
         <v>0.75</v>
       </c>
-      <c r="R8" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S8" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="T8" s="13" t="s">
+      <c r="R8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T8" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="19">
+      <c r="A9" s="10">
         <v>44108</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S9" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="T9" s="13" t="s">
+      <c r="B9" s="13">
+        <v>60</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="13">
+        <v>25</v>
+      </c>
+      <c r="E9" s="14">
+        <v>80</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0</v>
+      </c>
+      <c r="G9" s="14">
+        <v>0</v>
+      </c>
+      <c r="H9" s="13">
+        <v>2</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
+      <c r="J9" s="13">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <v>3</v>
+      </c>
+      <c r="L9" s="13">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7">
+        <v>1</v>
+      </c>
+      <c r="N9" s="13">
+        <v>0</v>
+      </c>
+      <c r="O9" s="13">
+        <v>1</v>
+      </c>
+      <c r="P9" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="15">
+        <v>0.84375</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T9" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="19">
+      <c r="A10" s="10">
         <v>44109</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S10" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="T10" s="13" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T10" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="19">
+      <c r="A11" s="10">
         <v>44110</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S11" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="T11" s="13" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T11" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="19">
+      <c r="A12" s="10">
         <v>44111</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S12" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="T12" s="13" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T12" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="19">
+      <c r="A13" s="10">
         <v>44112</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S13" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="T13" s="13" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T13" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="19">
+      <c r="A14" s="10">
         <v>44113</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S14" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="T14" s="13" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T14" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="19">
+      <c r="A15" s="10">
         <v>44114</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S15" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="T15" s="13" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T15" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="19">
+      <c r="A16" s="10">
         <v>44115</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S16" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="T16" s="13" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T16" s="7" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1547,12 +1579,12 @@
       <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
@@ -1563,30 +1595,30 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="5" spans="1:6" ht="33" customHeight="1">
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6" ht="37" customHeight="1">
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
@@ -1597,84 +1629,84 @@
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
     </row>
     <row r="9" spans="1:6" ht="29" customHeight="1">
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1">
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
     </row>
     <row r="11" spans="1:6" ht="33" customHeight="1">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:6" ht="33" customHeight="1">
       <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
     </row>
     <row r="14" spans="1:6" ht="33" customHeight="1">
       <c r="B14" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6" ht="33" customHeight="1">
       <c r="B15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
@@ -1685,30 +1717,30 @@
       <c r="B17" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
     </row>
     <row r="18" spans="1:6" ht="29" customHeight="1">
       <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
     </row>
     <row r="19" spans="1:6" ht="31" customHeight="1">
       <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
@@ -1719,34 +1751,34 @@
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
     </row>
     <row r="22" spans="1:6" ht="88" customHeight="1">
       <c r="B22" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
     </row>
     <row r="23" spans="1:6" ht="90" customHeight="1">
       <c r="B23" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
@@ -1757,51 +1789,51 @@
       <c r="B25" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
     </row>
     <row r="26" spans="1:6" ht="66" customHeight="1">
       <c r="B26" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
     </row>
     <row r="27" spans="1:6" ht="52" customHeight="1">
       <c r="B27" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C2:F2"/>
     <mergeCell ref="C4:F6"/>
     <mergeCell ref="C8:F10"/>
     <mergeCell ref="C17:F19"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C27:F27"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1822,231 +1854,236 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="G2" s="10" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="G2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="16"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="32"/>
     </row>
     <row r="3" spans="1:12" ht="36" customHeight="1">
-      <c r="A3" s="10">
-        <v>0</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="6">
+        <v>0</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="G3" s="10">
-        <v>0</v>
-      </c>
-      <c r="H3" s="11" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
     </row>
     <row r="4" spans="1:12" ht="56" customHeight="1">
-      <c r="A4" s="10">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="G4" s="10">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="G4" s="6">
         <v>1</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
     </row>
     <row r="5" spans="1:12" ht="53" customHeight="1">
-      <c r="A5" s="10">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="G5" s="10">
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="G5" s="6">
         <v>2</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
     </row>
     <row r="6" spans="1:12" ht="50" customHeight="1">
-      <c r="A6" s="10">
+      <c r="A6" s="6">
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="G6" s="10">
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="G6" s="6">
         <v>3</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
     </row>
     <row r="7" spans="1:12" ht="66" customHeight="1">
-      <c r="A7" s="10">
+      <c r="A7" s="6">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="G7" s="10">
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="G7" s="6">
         <v>4</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
     </row>
     <row r="8" spans="1:12" ht="67" customHeight="1">
-      <c r="A8" s="10">
+      <c r="A8" s="6">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="G8" s="10">
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="G8" s="6">
         <v>5</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="10">
-        <v>0</v>
-      </c>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="6">
+        <v>0</v>
+      </c>
+      <c r="B12" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="10">
+      <c r="A13" s="6">
         <v>1</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="10">
+      <c r="A14" s="6">
         <v>2</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="10">
+      <c r="A15" s="6">
         <v>3</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="10">
+      <c r="A16" s="6">
         <v>4</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="10">
+      <c r="A17" s="6">
         <v>5</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="H2:L2"/>
@@ -2063,11 +2100,6 @@
     <mergeCell ref="H5:L5"/>
     <mergeCell ref="H6:L6"/>
     <mergeCell ref="H7:L7"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2095,26 +2127,26 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="187">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>44103</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="119">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>44105</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="51">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>44108</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="8" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding updated tracker informationand peer lesson materials
</commit_message>
<xml_diff>
--- a/visualize_yourself/factor_tracker/factor_tracker_v1.xlsx
+++ b/visualize_yourself/factor_tracker/factor_tracker_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zack/dat203_ccac/visualize_yourself/factor_tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C21D159-1772-8C4D-919F-EC257E696272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B982DEB8-31B4-4748-A54A-12DCF800A38B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28500" yWindow="660" windowWidth="25440" windowHeight="15000" xr2:uid="{A1BA6AF8-65AC-1A49-9373-6E2A5D38BDA9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15000" xr2:uid="{A1BA6AF8-65AC-1A49-9373-6E2A5D38BDA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Scales" sheetId="3" r:id="rId3"/>
     <sheet name="Log" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="73">
   <si>
     <t>Screen Time</t>
   </si>
@@ -249,9 +249,6 @@
     <t>Slept poorly and waking state is exhausted; no rest achieved</t>
   </si>
   <si>
-    <t>Slightly rested though kept waking/tossing turning</t>
-  </si>
-  <si>
     <t>Trouble falling asleep; two or more wakes. Could not get comfortable</t>
   </si>
   <si>
@@ -272,6 +269,20 @@
   <si>
     <t>Work done:
 * Transposed dataframe so that indeces are time series not factors</t>
+  </si>
+  <si>
+    <t>Screen Time (previous night)</t>
+  </si>
+  <si>
+    <t>Reading print (previous night)</t>
+  </si>
+  <si>
+    <t>Work done:
+* Updated sleep scale values to be more specific</t>
+  </si>
+  <si>
+    <t>Basic function of sleep to recharge satisfied though kept waking/tossing turning;
+quality of sleep does not result in recharge but merely enough to keep going</t>
   </si>
 </sst>
 </file>
@@ -448,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -527,6 +538,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -842,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E573A9E-18A6-FA42-859D-81536E76F4F6}">
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -868,12 +882,12 @@
         <v>20</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
       <c r="E2" s="23" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="F2" s="24"/>
       <c r="G2" s="25"/>
@@ -1139,13 +1153,13 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1201,13 +1215,13 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1263,13 +1277,13 @@
         <v>0.75</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1325,223 +1339,1031 @@
         <v>0.84375</v>
       </c>
       <c r="R9" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="10">
         <v>44109</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="13"/>
+      <c r="B10" s="13">
+        <v>60</v>
+      </c>
+      <c r="C10" s="7">
+        <v>15</v>
+      </c>
+      <c r="D10" s="13">
+        <v>30</v>
+      </c>
+      <c r="E10" s="14">
+        <v>60</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0</v>
+      </c>
+      <c r="H10" s="13">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
+        <v>2</v>
+      </c>
+      <c r="J10" s="13">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <v>2</v>
+      </c>
+      <c r="L10" s="13">
+        <v>1</v>
+      </c>
+      <c r="M10" s="7">
+        <v>1</v>
+      </c>
+      <c r="N10" s="13">
+        <v>0</v>
+      </c>
+      <c r="O10" s="13">
+        <v>2</v>
+      </c>
+      <c r="P10" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="15">
+        <v>0.875</v>
+      </c>
       <c r="R10" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S10" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="10">
         <v>44110</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="13"/>
+      <c r="B11" s="13">
+        <v>45</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="13">
+        <v>35</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0</v>
+      </c>
+      <c r="G11" s="14">
+        <v>0</v>
+      </c>
+      <c r="H11" s="13">
+        <v>2</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0</v>
+      </c>
+      <c r="J11" s="13">
+        <v>1</v>
+      </c>
+      <c r="K11" s="7">
+        <v>3</v>
+      </c>
+      <c r="L11" s="13">
+        <v>0</v>
+      </c>
+      <c r="M11" s="7">
+        <v>0</v>
+      </c>
+      <c r="N11" s="13">
+        <v>0</v>
+      </c>
+      <c r="O11" s="13">
+        <v>2</v>
+      </c>
+      <c r="P11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="15">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="R11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="10">
         <v>44111</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="13"/>
+      <c r="B12" s="13">
+        <v>45</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="13">
+        <v>20</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0</v>
+      </c>
+      <c r="H12" s="13">
+        <v>2</v>
+      </c>
+      <c r="I12" s="7">
+        <v>1</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0</v>
+      </c>
+      <c r="K12" s="7">
+        <v>2</v>
+      </c>
+      <c r="L12" s="13">
+        <v>2</v>
+      </c>
+      <c r="M12" s="7">
+        <v>1</v>
+      </c>
+      <c r="N12" s="13">
+        <v>0</v>
+      </c>
+      <c r="O12" s="13">
+        <v>4</v>
+      </c>
+      <c r="P12" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="15">
+        <v>0.8125</v>
+      </c>
       <c r="R12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="10">
         <v>44112</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="13"/>
+      <c r="B13" s="13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>150</v>
+      </c>
+      <c r="D13" s="13">
+        <v>15</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="14">
+        <v>0</v>
+      </c>
+      <c r="H13" s="13">
+        <v>2</v>
+      </c>
+      <c r="I13" s="7">
+        <v>1</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
+        <v>2</v>
+      </c>
+      <c r="L13" s="13">
+        <v>1</v>
+      </c>
+      <c r="M13" s="7">
+        <v>1</v>
+      </c>
+      <c r="N13" s="13">
+        <v>0</v>
+      </c>
+      <c r="O13" s="13">
+        <v>3</v>
+      </c>
+      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="15">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="R13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="10">
         <v>44113</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="13"/>
+      <c r="B14" s="13">
+        <v>60</v>
+      </c>
+      <c r="C14" s="7">
+        <v>60</v>
+      </c>
+      <c r="D14" s="13">
+        <v>0</v>
+      </c>
+      <c r="E14" s="14">
+        <v>60</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <v>1</v>
+      </c>
+      <c r="K14" s="7">
+        <v>3</v>
+      </c>
+      <c r="L14" s="13">
+        <v>3</v>
+      </c>
+      <c r="M14" s="7">
+        <v>2</v>
+      </c>
+      <c r="N14" s="13">
+        <v>0</v>
+      </c>
+      <c r="O14" s="13">
+        <v>2</v>
+      </c>
+      <c r="P14" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="15">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="R14" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="10">
         <v>44114</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="13"/>
+      <c r="B15" s="13">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7">
+        <v>120</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0</v>
+      </c>
+      <c r="F15" s="13">
+        <v>0</v>
+      </c>
+      <c r="G15" s="14">
+        <v>0</v>
+      </c>
+      <c r="H15" s="13">
+        <v>2</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
+        <v>2</v>
+      </c>
+      <c r="L15" s="13">
+        <v>3</v>
+      </c>
+      <c r="M15" s="7">
+        <v>3</v>
+      </c>
+      <c r="N15" s="13">
+        <v>0</v>
+      </c>
+      <c r="O15" s="13">
+        <v>2</v>
+      </c>
+      <c r="P15" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="15">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="R15" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S15" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="10">
         <v>44115</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="13"/>
+      <c r="B16" s="13">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>180</v>
+      </c>
+      <c r="D16" s="13">
+        <v>15</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0</v>
+      </c>
+      <c r="F16" s="13">
+        <v>0</v>
+      </c>
+      <c r="G16" s="14">
+        <v>0</v>
+      </c>
+      <c r="H16" s="13">
+        <v>1</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0</v>
+      </c>
+      <c r="J16" s="13">
+        <v>0</v>
+      </c>
+      <c r="K16" s="7">
+        <v>2</v>
+      </c>
+      <c r="L16" s="13">
+        <v>2</v>
+      </c>
+      <c r="M16" s="7">
+        <v>2</v>
+      </c>
+      <c r="N16" s="13">
+        <v>0</v>
+      </c>
+      <c r="O16" s="13">
+        <v>1</v>
+      </c>
+      <c r="P16" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="15">
+        <v>0.875</v>
+      </c>
       <c r="R16" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="10">
+        <v>44116</v>
+      </c>
+      <c r="B17" s="13">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7">
+        <v>90</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0</v>
+      </c>
+      <c r="E17" s="14">
+        <v>0</v>
+      </c>
+      <c r="F17" s="13">
+        <v>0</v>
+      </c>
+      <c r="G17" s="14">
+        <v>0</v>
+      </c>
+      <c r="H17" s="13">
+        <v>1</v>
+      </c>
+      <c r="I17" s="7">
+        <v>3</v>
+      </c>
+      <c r="J17" s="13">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7">
+        <v>2</v>
+      </c>
+      <c r="L17" s="13">
+        <v>3</v>
+      </c>
+      <c r="M17" s="7">
+        <v>1</v>
+      </c>
+      <c r="N17" s="13">
+        <v>0</v>
+      </c>
+      <c r="O17" s="13">
+        <v>1</v>
+      </c>
+      <c r="P17" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="15">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="10">
+        <v>44117</v>
+      </c>
+      <c r="B18" s="13">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7">
+        <v>120</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0</v>
+      </c>
+      <c r="E18" s="14">
+        <v>0</v>
+      </c>
+      <c r="F18" s="13">
+        <v>0</v>
+      </c>
+      <c r="G18" s="14">
+        <v>0</v>
+      </c>
+      <c r="H18" s="13">
+        <v>1</v>
+      </c>
+      <c r="I18" s="7">
+        <v>3</v>
+      </c>
+      <c r="J18" s="13">
+        <v>0</v>
+      </c>
+      <c r="K18" s="7">
+        <v>2</v>
+      </c>
+      <c r="L18" s="13">
+        <v>3</v>
+      </c>
+      <c r="M18" s="7">
+        <v>2</v>
+      </c>
+      <c r="N18" s="13">
+        <v>0</v>
+      </c>
+      <c r="O18" s="13">
+        <v>2</v>
+      </c>
+      <c r="P18" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="15">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="10">
+        <v>44118</v>
+      </c>
+      <c r="B19" s="13">
+        <v>60</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0</v>
+      </c>
+      <c r="E19" s="14">
+        <v>35</v>
+      </c>
+      <c r="F19" s="13">
+        <v>0</v>
+      </c>
+      <c r="G19" s="14">
+        <v>0</v>
+      </c>
+      <c r="H19" s="13">
+        <v>2</v>
+      </c>
+      <c r="I19" s="7">
+        <v>2</v>
+      </c>
+      <c r="J19" s="13">
+        <v>0</v>
+      </c>
+      <c r="K19" s="7">
+        <v>2</v>
+      </c>
+      <c r="L19" s="13">
+        <v>2</v>
+      </c>
+      <c r="M19" s="7">
+        <v>2</v>
+      </c>
+      <c r="N19" s="13">
+        <v>0</v>
+      </c>
+      <c r="O19" s="13">
+        <v>1</v>
+      </c>
+      <c r="P19" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="15">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T19" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="10">
+        <v>44119</v>
+      </c>
+      <c r="B20" s="13">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7">
+        <v>180</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0</v>
+      </c>
+      <c r="E20" s="14">
+        <v>0</v>
+      </c>
+      <c r="F20" s="13">
+        <v>0</v>
+      </c>
+      <c r="G20" s="14">
+        <v>0</v>
+      </c>
+      <c r="H20" s="13">
+        <v>2</v>
+      </c>
+      <c r="I20" s="7">
+        <v>1</v>
+      </c>
+      <c r="J20" s="13">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7">
+        <v>2</v>
+      </c>
+      <c r="L20" s="13">
+        <v>3</v>
+      </c>
+      <c r="M20" s="7">
+        <v>2</v>
+      </c>
+      <c r="N20" s="13">
+        <v>0</v>
+      </c>
+      <c r="O20" s="13">
+        <v>2</v>
+      </c>
+      <c r="P20" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="15">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="R20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T20" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="10">
+        <v>44120</v>
+      </c>
+      <c r="B21" s="13">
+        <v>60</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0</v>
+      </c>
+      <c r="E21" s="14">
+        <v>15</v>
+      </c>
+      <c r="F21" s="13">
+        <v>0</v>
+      </c>
+      <c r="G21" s="14">
+        <v>0</v>
+      </c>
+      <c r="H21" s="13">
+        <v>2</v>
+      </c>
+      <c r="I21" s="7">
+        <v>1</v>
+      </c>
+      <c r="J21" s="13">
+        <v>0</v>
+      </c>
+      <c r="K21" s="7">
+        <v>2</v>
+      </c>
+      <c r="L21" s="13">
+        <v>2</v>
+      </c>
+      <c r="M21" s="7">
+        <v>3</v>
+      </c>
+      <c r="N21" s="13">
+        <v>0</v>
+      </c>
+      <c r="O21" s="13">
+        <v>2</v>
+      </c>
+      <c r="P21" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="15">
+        <v>0.8125</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T21" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="10">
+        <v>44121</v>
+      </c>
+      <c r="B22" s="13">
+        <v>120</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0</v>
+      </c>
+      <c r="D22" s="13">
+        <v>15</v>
+      </c>
+      <c r="E22" s="14">
+        <v>15</v>
+      </c>
+      <c r="F22" s="13">
+        <v>0</v>
+      </c>
+      <c r="G22" s="14">
+        <v>0</v>
+      </c>
+      <c r="H22" s="13">
+        <v>2</v>
+      </c>
+      <c r="I22" s="7">
+        <v>1</v>
+      </c>
+      <c r="J22" s="13">
+        <v>0</v>
+      </c>
+      <c r="K22" s="7">
+        <v>2</v>
+      </c>
+      <c r="L22" s="13">
+        <v>2</v>
+      </c>
+      <c r="M22" s="7">
+        <v>3</v>
+      </c>
+      <c r="N22" s="13">
+        <v>0</v>
+      </c>
+      <c r="O22" s="13">
+        <v>2</v>
+      </c>
+      <c r="P22" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="15">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S22" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="10">
+        <v>44122</v>
+      </c>
+      <c r="B23" s="13">
+        <v>0</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0</v>
+      </c>
+      <c r="E23" s="14">
+        <v>0</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0</v>
+      </c>
+      <c r="G23" s="14">
+        <v>0</v>
+      </c>
+      <c r="H23" s="13">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7">
+        <v>0</v>
+      </c>
+      <c r="J23" s="13">
+        <v>0</v>
+      </c>
+      <c r="K23" s="7">
+        <v>3</v>
+      </c>
+      <c r="L23" s="13">
+        <v>2</v>
+      </c>
+      <c r="M23" s="7">
+        <v>3</v>
+      </c>
+      <c r="N23" s="13">
+        <v>0</v>
+      </c>
+      <c r="O23" s="13">
+        <v>3</v>
+      </c>
+      <c r="P23" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="15">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="10">
+        <v>44123</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S24" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T24" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="10">
+        <v>44124</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="10">
+        <v>44125</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S26" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="10">
+        <v>44126</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T27" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="10">
+        <v>44127</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T28" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1844,7 +2666,7 @@
   <dimension ref="A2:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:E17"/>
+      <selection activeCell="B13" sqref="B13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2033,12 +2855,12 @@
       <c r="D13" s="29"/>
       <c r="E13" s="29"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="6">
         <v>2</v>
       </c>
-      <c r="B14" s="29" t="s">
-        <v>63</v>
+      <c r="B14" s="35" t="s">
+        <v>72</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
@@ -2049,7 +2871,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="29"/>
@@ -2060,7 +2882,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
@@ -2071,7 +2893,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
@@ -2107,10 +2929,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1339649-4464-704C-9B3C-8EA194FC3F4C}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2139,7 +2961,7 @@
         <v>44105</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="51">
@@ -2147,7 +2969,15 @@
         <v>44108</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="34">
+      <c r="A5" s="3">
+        <v>44119</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>